<commit_message>
Added framework design Context explanation
</commit_message>
<xml_diff>
--- a/src/main/resources/userData.xlsx
+++ b/src/main/resources/userData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgundalaA/RestAssured/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78DFEBA2-284D-2E42-A1E1-4A5690D99F2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF93AEB-3652-AC46-9665-802A23F55F60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{EA3458B9-62D9-DD45-BF99-C2BD5A0D4C2B}"/>
   </bookViews>
@@ -69,10 +69,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -95,13 +103,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -416,7 +427,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8A3F19-5A71-F04A-B83E-6F8650FE66C3}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -432,7 +445,7 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -461,6 +474,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="leader@cell$12@1" xr:uid="{06886C0B-2079-8243-9EF8-C2B4C8E3FC02}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>